<commit_message>
added src/test/java as this is needed for maven
Signed-off-by: rajp <rajp@WIN-VQNIP6TPSR5.localdomain>
</commit_message>
<xml_diff>
--- a/Beton/data/testResults.xlsx
+++ b/Beton/data/testResults.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="null" r:id="rId5" sheetId="2"/>
+    <sheet name="iPhone-6 Raj" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Test Parameters</t>
   </si>
@@ -92,12 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,4 +449,33 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>